<commit_message>
[Fix]: update calculations dir
</commit_message>
<xml_diff>
--- a/calculations/LMN_norm.xlsx
+++ b/calculations/LMN_norm.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Training" sheetId="1" state="visible" r:id="rId2"/>
@@ -198,6 +198,1296 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="184">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB4C7E7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF63BE7B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF66BF7B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7FC67C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF91CB7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9ACE7E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFADD37F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFBCD780"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFBED880"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DB80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD8DF81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF1E683"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF7E883"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8696B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9786E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDC37D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDC67D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFECC7E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFED680"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFED781"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFDB81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFDD82"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE283"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE483"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEA84"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB84"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF96CC7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9CCE7E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FCF7E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA2D07E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFABD27F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6DA80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCADB80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2E282"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE6E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFA8E72"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFB9173"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDBB7B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFED07F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFED280"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFED380"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFD981"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE182"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE984"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA9D27F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCEDC81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDAE081"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE8E482"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE9E482"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEEE683"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF6E883"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9E983"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCA677"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCAB78"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDB77A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEC97E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFED17F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8FCA7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF93CC7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7D67F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC7DB80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDCE081"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDDE182"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE4E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF0E683"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDBE7C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFECE7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFDC81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFDC82"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE383"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE784"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF90CB7E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF94CD7E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA3D17F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8D780"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC8DC81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDEE283"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE5E483"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF1E784"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF7E984"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCBD7B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCC27C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDCD7E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEDB80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEDB81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEE081"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEE282"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEE382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEE683"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEE883"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEEA83"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF97CD7E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA6D27F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB9D780"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCADC81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E082"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE1E383"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3E884"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBEA84"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCBE7B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCC47C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDEB84"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEDD81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEDE81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEE182"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEE482"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEE983"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6DC07B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6EC17B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6FC17B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF73C27B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0DD81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEAE482"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEAE582"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9746D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBEA83"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCA477"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCAD78"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDC27C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFECB7E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFED580"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF71C27B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF74C37C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF79C47C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7DC57C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF81C67C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF83C77C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF88C87D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE7E482"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF96D6C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFA8070"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFA8571"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE183"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE683"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE684"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF76C37C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF82C67C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8DCA7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA5D17E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEDE683"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFA8270"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFA8370"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFB9874"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFB9D75"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDEA83"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFDF82"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE583"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE884"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF75C37C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8CC97D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA3D07E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFAAD27F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCFDD81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEDE582"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFA8471"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFA8671"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFB9C75"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCA176"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE082"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF76C47D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF82C77D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8DCA7E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA4D17F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFABD380"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0DE82"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEAE583"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF98370"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF98570"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFA9B74"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFAEA84"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBA075"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEDF81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEEB84"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF73C37C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA0D07F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCDD82"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF2E884"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9826F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF98770"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBA676"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCEB84"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEE582"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEE783"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -276,11 +1566,11 @@
   </sheetPr>
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="1" style="1" width="12.71"/>
   </cols>
@@ -1040,7 +2330,7 @@
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1056,11 +2346,11 @@
   </sheetPr>
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="1" style="1" width="12.71"/>
   </cols>
@@ -1818,7 +3108,7 @@
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Update project structure (#14)
* [Feature]: create a shell script to build a project environment

* [Feature]: initialize pre-commit

* [Fix]: remove unnecessary files and packages

* [Fix]: move SHAP integration from the main branch

* [Fix]: update calculations dir

* [Feature]: add demo dataset

* [Feature]: add predictions for both models

* [Fix]: add gitkeep files to main project directories

* [Fix]: update default values

* [Fix]: include experiments for tracking

* [Fix]: add experiment artifacts

* [Feature]: initialize DVC storage

* [Feature]: upload models to DVC
</commit_message>
<xml_diff>
--- a/calculations/LMN_norm.xlsx
+++ b/calculations/LMN_norm.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Training" sheetId="1" state="visible" r:id="rId2"/>
@@ -198,6 +198,1296 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="184">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB4C7E7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF63BE7B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF66BF7B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7FC67C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF91CB7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9ACE7E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFADD37F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFBCD780"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFBED880"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DB80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD8DF81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF1E683"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF7E883"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8696B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9786E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDC37D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDC67D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFECC7E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFED680"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFED781"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFDB81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFDD82"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE283"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE483"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEA84"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB84"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF96CC7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9CCE7E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9FCF7E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA2D07E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFABD27F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6DA80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCADB80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2E282"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE6E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFA8E72"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFB9173"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDBB7B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFED07F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFED280"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFED380"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFD981"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE182"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE984"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA9D27F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCEDC81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDAE081"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE8E482"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE9E482"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEEE683"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF6E883"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9E983"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCA677"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCAB78"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDB77A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEC97E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFED17F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8FCA7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF93CC7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7D67F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC7DB80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDCE081"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDDE182"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE4E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF0E683"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDBE7C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFECE7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFDC81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFDC82"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE383"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE784"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF90CB7E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF94CD7E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA3D17F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8D780"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC8DC81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDEE283"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE5E483"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF1E784"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF7E984"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCBD7B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCC27C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDCD7E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEDB80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEDB81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEE081"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEE282"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEE382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEE683"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEE883"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEEA83"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF97CD7E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA6D27F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB9D780"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCADC81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E082"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE1E383"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3E884"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBEA84"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCBE7B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCC47C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDEB84"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEDD81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEDE81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEE182"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEE482"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEE983"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6DC07B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6EC17B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6FC17B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF73C27B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0DD81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEAE482"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEAE582"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9746D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBEA83"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCA477"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCAD78"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDC27C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFECB7E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFED580"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF71C27B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF74C37C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF79C47C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7DC57C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF81C67C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF83C77C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF88C87D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE7E482"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF96D6C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFA8070"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFA8571"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE183"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE683"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE684"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF76C37C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF82C67C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8DCA7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA5D17E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEDE683"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFA8270"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFA8370"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFB9874"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFB9D75"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDEA83"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFDF82"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE583"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE884"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF75C37C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8CC97D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA3D07E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFAAD27F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCFDD81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEDE582"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFA8471"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFA8671"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFB9C75"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCA176"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE082"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF76C47D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF82C77D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8DCA7E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA4D17F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFABD380"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0DE82"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEAE583"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF98370"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF98570"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFA9B74"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFAEA84"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBA075"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEDF81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEEB84"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF73C37C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA0D07F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCDD82"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF2E884"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9826F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF98770"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBA676"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCEB84"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEE582"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEE783"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -276,11 +1566,11 @@
   </sheetPr>
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="1" style="1" width="12.71"/>
   </cols>
@@ -1040,7 +2330,7 @@
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1056,11 +2346,11 @@
   </sheetPr>
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="1" style="1" width="12.71"/>
   </cols>
@@ -1818,7 +3108,7 @@
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>